<commit_message>
Update the results collected
</commit_message>
<xml_diff>
--- a/Open day poster/Project Results Form II.xlsx
+++ b/Open day poster/Project Results Form II.xlsx
@@ -332,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -401,11 +401,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -473,6 +482,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -822,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -912,33 +922,33 @@
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15.75">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="45" t="s">
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47" t="s">
+      <c r="H7" s="47"/>
+      <c r="I7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="50"/>
     </row>
     <row r="8" spans="1:11" ht="34.5" customHeight="1">
-      <c r="A8" s="50"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="7" t="s">
         <v>16</v>
       </c>
@@ -950,13 +960,13 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="12" customFormat="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="30"/>
       <c r="G9" s="34">
         <v>2</v>
@@ -973,13 +983,13 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
       <c r="F10" s="33"/>
       <c r="G10" s="18">
         <v>2</v>
@@ -1012,13 +1022,13 @@
       </c>
     </row>
     <row r="12" spans="1:11" s="13" customFormat="1">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
       <c r="F12" s="30"/>
       <c r="G12" s="34">
         <v>1</v>
@@ -1035,13 +1045,13 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="13" customFormat="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
       <c r="F13" s="30"/>
       <c r="G13" s="34">
         <v>2</v>
@@ -1058,13 +1068,13 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="13" customFormat="1">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
       <c r="F14" s="30"/>
       <c r="G14" s="34">
         <v>0</v>
@@ -1078,6 +1088,23 @@
       </c>
       <c r="K14" s="16">
         <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="G15" s="43">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <f>I9+I10+I14</f>
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <f>J10+J13+J14</f>
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <f>K9+K10+K12+K13+K14</f>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1294,33 +1321,33 @@
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:11" ht="15.75">
-      <c r="A54" s="54" t="s">
+      <c r="A54" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="53"/>
-      <c r="G54" s="45" t="s">
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H54" s="46"/>
-      <c r="I54" s="47" t="s">
+      <c r="H54" s="47"/>
+      <c r="I54" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="J54" s="48"/>
-      <c r="K54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="50"/>
     </row>
     <row r="55" spans="1:11" ht="30">
-      <c r="A55" s="50"/>
-      <c r="B55" s="52"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="51"/>
+      <c r="A55" s="51"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="52"/>
       <c r="I55" s="7" t="s">
         <v>16</v>
       </c>
@@ -1332,13 +1359,13 @@
       </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="43" t="s">
+      <c r="A56" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
+      <c r="B56" s="45"/>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
       <c r="F56" s="30"/>
       <c r="G56" s="34"/>
       <c r="H56" s="30"/>
@@ -1353,13 +1380,13 @@
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B57" s="57"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
-      <c r="E57" s="57"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
       <c r="F57" s="33"/>
       <c r="G57" s="18"/>
       <c r="H57" s="33"/>
@@ -1431,13 +1458,13 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J61" s="38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K61" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -1689,33 +1716,33 @@
       <c r="I101" s="1"/>
     </row>
     <row r="102" spans="1:11" ht="15.75">
-      <c r="A102" s="54" t="s">
+      <c r="A102" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="55"/>
-      <c r="C102" s="55"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="44"/>
-      <c r="F102" s="53"/>
-      <c r="G102" s="45" t="s">
+      <c r="B102" s="56"/>
+      <c r="C102" s="56"/>
+      <c r="D102" s="45"/>
+      <c r="E102" s="45"/>
+      <c r="F102" s="54"/>
+      <c r="G102" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H102" s="46"/>
-      <c r="I102" s="47" t="s">
+      <c r="H102" s="47"/>
+      <c r="I102" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="J102" s="48"/>
-      <c r="K102" s="49"/>
+      <c r="J102" s="49"/>
+      <c r="K102" s="50"/>
     </row>
     <row r="103" spans="1:11" ht="30">
-      <c r="A103" s="50"/>
-      <c r="B103" s="52"/>
-      <c r="C103" s="52"/>
-      <c r="D103" s="52"/>
-      <c r="E103" s="52"/>
-      <c r="F103" s="53"/>
-      <c r="G103" s="50"/>
-      <c r="H103" s="51"/>
+      <c r="A103" s="51"/>
+      <c r="B103" s="53"/>
+      <c r="C103" s="53"/>
+      <c r="D103" s="53"/>
+      <c r="E103" s="53"/>
+      <c r="F103" s="54"/>
+      <c r="G103" s="51"/>
+      <c r="H103" s="52"/>
       <c r="I103" s="7" t="s">
         <v>16</v>
       </c>
@@ -1727,18 +1754,18 @@
       </c>
     </row>
     <row r="104" spans="1:11">
-      <c r="A104" s="43" t="s">
+      <c r="A104" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B104" s="44"/>
-      <c r="C104" s="44"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="44"/>
+      <c r="B104" s="45"/>
+      <c r="C104" s="45"/>
+      <c r="D104" s="45"/>
+      <c r="E104" s="45"/>
       <c r="F104" s="11"/>
-      <c r="G104" s="58">
+      <c r="G104" s="59">
         <v>0</v>
       </c>
-      <c r="H104" s="59"/>
+      <c r="H104" s="60"/>
       <c r="I104" s="39">
         <v>10</v>
       </c>
@@ -1750,18 +1777,18 @@
       </c>
     </row>
     <row r="105" spans="1:11">
-      <c r="A105" s="56" t="s">
+      <c r="A105" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="B105" s="57"/>
-      <c r="C105" s="57"/>
-      <c r="D105" s="57"/>
-      <c r="E105" s="57"/>
+      <c r="B105" s="58"/>
+      <c r="C105" s="58"/>
+      <c r="D105" s="58"/>
+      <c r="E105" s="58"/>
       <c r="F105" s="14"/>
-      <c r="G105" s="60">
+      <c r="G105" s="61">
         <v>0</v>
       </c>
-      <c r="H105" s="61"/>
+      <c r="H105" s="62"/>
       <c r="I105" s="40">
         <v>14</v>
       </c>
@@ -1804,8 +1831,8 @@
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
       <c r="H108" s="22"/>
-      <c r="I108" s="64"/>
-      <c r="J108" s="64"/>
+      <c r="I108" s="65"/>
+      <c r="J108" s="65"/>
     </row>
     <row r="109" spans="1:11">
       <c r="C109" s="3">
@@ -1887,18 +1914,18 @@
       <c r="K116" s="24"/>
     </row>
     <row r="117" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A117" s="65" t="s">
+      <c r="A117" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B117" s="63"/>
-      <c r="C117" s="63"/>
-      <c r="D117" s="63"/>
-      <c r="E117" s="63"/>
-      <c r="F117" s="63"/>
-      <c r="G117" s="63"/>
-      <c r="H117" s="63"/>
-      <c r="I117" s="63"/>
-      <c r="J117" s="63"/>
+      <c r="B117" s="64"/>
+      <c r="C117" s="64"/>
+      <c r="D117" s="64"/>
+      <c r="E117" s="64"/>
+      <c r="F117" s="64"/>
+      <c r="G117" s="64"/>
+      <c r="H117" s="64"/>
+      <c r="I117" s="64"/>
+      <c r="J117" s="64"/>
     </row>
     <row r="118" spans="1:11">
       <c r="C118" s="3">
@@ -2015,18 +2042,18 @@
       <c r="J130" s="6"/>
     </row>
     <row r="132" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A132" s="62" t="s">
+      <c r="A132" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="62"/>
-      <c r="C132" s="62"/>
-      <c r="D132" s="62"/>
-      <c r="E132" s="62"/>
-      <c r="F132" s="62"/>
-      <c r="G132" s="62"/>
-      <c r="H132" s="62"/>
-      <c r="I132" s="62"/>
-      <c r="J132" s="62"/>
+      <c r="B132" s="63"/>
+      <c r="C132" s="63"/>
+      <c r="D132" s="63"/>
+      <c r="E132" s="63"/>
+      <c r="F132" s="63"/>
+      <c r="G132" s="63"/>
+      <c r="H132" s="63"/>
+      <c r="I132" s="63"/>
+      <c r="J132" s="63"/>
     </row>
     <row r="133" spans="1:11">
       <c r="C133" s="3">
@@ -2070,18 +2097,18 @@
       <c r="K135" s="24"/>
     </row>
     <row r="136" spans="1:11" ht="33" customHeight="1">
-      <c r="A136" s="62" t="s">
+      <c r="A136" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="B136" s="63"/>
-      <c r="C136" s="63"/>
-      <c r="D136" s="63"/>
-      <c r="E136" s="63"/>
-      <c r="F136" s="63"/>
-      <c r="G136" s="63"/>
-      <c r="H136" s="63"/>
-      <c r="I136" s="63"/>
-      <c r="J136" s="63"/>
+      <c r="B136" s="64"/>
+      <c r="C136" s="64"/>
+      <c r="D136" s="64"/>
+      <c r="E136" s="64"/>
+      <c r="F136" s="64"/>
+      <c r="G136" s="64"/>
+      <c r="H136" s="64"/>
+      <c r="I136" s="64"/>
+      <c r="J136" s="64"/>
     </row>
     <row r="137" spans="1:11">
       <c r="C137" s="3">
@@ -2122,18 +2149,18 @@
       <c r="J139" s="6"/>
     </row>
     <row r="140" spans="1:11" ht="29.25" customHeight="1">
-      <c r="A140" s="62" t="s">
+      <c r="A140" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="B140" s="63"/>
-      <c r="C140" s="63"/>
-      <c r="D140" s="63"/>
-      <c r="E140" s="63"/>
-      <c r="F140" s="63"/>
-      <c r="G140" s="63"/>
-      <c r="H140" s="63"/>
-      <c r="I140" s="63"/>
-      <c r="J140" s="63"/>
+      <c r="B140" s="64"/>
+      <c r="C140" s="64"/>
+      <c r="D140" s="64"/>
+      <c r="E140" s="64"/>
+      <c r="F140" s="64"/>
+      <c r="G140" s="64"/>
+      <c r="H140" s="64"/>
+      <c r="I140" s="64"/>
+      <c r="J140" s="64"/>
     </row>
     <row r="141" spans="1:11">
       <c r="C141" s="3">
@@ -2169,18 +2196,18 @@
       <c r="K142" s="24"/>
     </row>
     <row r="143" spans="1:11" ht="61.5" customHeight="1">
-      <c r="A143" s="62" t="s">
+      <c r="A143" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B143" s="62"/>
-      <c r="C143" s="62"/>
-      <c r="D143" s="62"/>
-      <c r="E143" s="62"/>
-      <c r="F143" s="62"/>
-      <c r="G143" s="62"/>
-      <c r="H143" s="62"/>
-      <c r="I143" s="62"/>
-      <c r="J143" s="62"/>
+      <c r="B143" s="63"/>
+      <c r="C143" s="63"/>
+      <c r="D143" s="63"/>
+      <c r="E143" s="63"/>
+      <c r="F143" s="63"/>
+      <c r="G143" s="63"/>
+      <c r="H143" s="63"/>
+      <c r="I143" s="63"/>
+      <c r="J143" s="63"/>
     </row>
     <row r="144" spans="1:11">
       <c r="C144" s="3">
@@ -2266,18 +2293,18 @@
       <c r="J150" s="6"/>
     </row>
     <row r="152" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A152" s="62" t="s">
+      <c r="A152" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="B152" s="63"/>
-      <c r="C152" s="63"/>
-      <c r="D152" s="63"/>
-      <c r="E152" s="63"/>
-      <c r="F152" s="63"/>
-      <c r="G152" s="63"/>
-      <c r="H152" s="63"/>
-      <c r="I152" s="63"/>
-      <c r="J152" s="63"/>
+      <c r="B152" s="64"/>
+      <c r="C152" s="64"/>
+      <c r="D152" s="64"/>
+      <c r="E152" s="64"/>
+      <c r="F152" s="64"/>
+      <c r="G152" s="64"/>
+      <c r="H152" s="64"/>
+      <c r="I152" s="64"/>
+      <c r="J152" s="64"/>
     </row>
     <row r="153" spans="1:11">
       <c r="C153" s="3">

</xml_diff>